<commit_message>
DHW and survivorship curves
</commit_message>
<xml_diff>
--- a/environmental_data/raw_data/Allyson-full-metadata.xlsx
+++ b/environmental_data/raw_data/Allyson-full-metadata.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.jankulak/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch3_reciprocaltransplant/environmental_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64C5598-787D-4C49-B09F-46C153A15B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{D64C5598-787D-4C49-B09F-46C153A15B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD41708B-BE22-8A42-9990-09A78C9F22CD}"/>
   <bookViews>
-    <workbookView xWindow="20300" yWindow="2040" windowWidth="28040" windowHeight="17440" xr2:uid="{9F59E8B1-1EC7-6644-80C6-299F852C6A5D}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{9F59E8B1-1EC7-6644-80C6-299F852C6A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -135,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,6 +162,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -221,19 +226,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -255,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,13 +558,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8835C3E-E97E-664C-A1A3-D0219CDE0169}">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="L23" sqref="G18:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,34 +576,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="4" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="4" t="s">
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -700,7 +707,7 @@
       <c r="U3" s="1">
         <v>45250</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -735,7 +742,7 @@
       <c r="U4" s="1">
         <v>45250</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="V4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -755,7 +762,7 @@
       <c r="F5" s="1">
         <v>45247</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="2"/>
@@ -768,7 +775,7 @@
       <c r="K5" s="1">
         <v>45013</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="2"/>
@@ -781,7 +788,7 @@
       <c r="P5" s="1">
         <v>45118</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="R5" s="2"/>
@@ -794,7 +801,7 @@
       <c r="U5" s="1">
         <v>45250</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="V5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -814,7 +821,7 @@
       <c r="F6" s="1">
         <v>45247</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="1">
@@ -829,7 +836,7 @@
       <c r="K6" s="1">
         <v>45013</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M6" s="1">
@@ -844,7 +851,7 @@
       <c r="P6" s="1">
         <v>45118</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="R6" s="1">
@@ -859,7 +866,7 @@
       <c r="U6" s="1">
         <v>45250</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="V6" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -879,7 +886,7 @@
       <c r="F7" s="1">
         <v>45247</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="1">
@@ -894,7 +901,7 @@
       <c r="K7" s="1">
         <v>45013</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M7" s="1">
@@ -909,7 +916,7 @@
       <c r="P7" s="1">
         <v>45118</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="R7" s="1">
@@ -924,7 +931,7 @@
       <c r="U7" s="1">
         <v>45250</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="V7" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -962,7 +969,7 @@
       <c r="U8" s="1">
         <v>45250</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="V8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -997,7 +1004,7 @@
       <c r="U9" s="1">
         <v>45250</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="V9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1017,7 +1024,7 @@
       <c r="F10" s="1">
         <v>45247</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="2"/>
@@ -1030,7 +1037,7 @@
       <c r="K10" s="1">
         <v>45013</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M10" s="2"/>
@@ -1043,7 +1050,7 @@
       <c r="P10" s="1">
         <v>45118</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="R10" s="2"/>
@@ -1056,7 +1063,7 @@
       <c r="U10" s="1">
         <v>45250</v>
       </c>
-      <c r="V10" s="7" t="s">
+      <c r="V10" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1076,7 +1083,7 @@
       <c r="F11" s="1">
         <v>45247</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="1">
@@ -1091,7 +1098,7 @@
       <c r="K11" s="1">
         <v>45013</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M11" s="1">
@@ -1106,7 +1113,7 @@
       <c r="P11" s="1">
         <v>45118</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="R11" s="1">
@@ -1141,7 +1148,7 @@
       <c r="F12" s="1">
         <v>45247</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="1">
@@ -1156,7 +1163,7 @@
       <c r="K12" s="1">
         <v>45013</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M12" s="1">
@@ -1186,9 +1193,37 @@
       <c r="U12" s="1">
         <v>45250</v>
       </c>
-      <c r="V12" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="V12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G19" s="9"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G20" s="9"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G21" s="9"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G22" s="9"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>